<commit_message>
Added PersonPII graph and trans files
</commit_message>
<xml_diff>
--- a/Fusion/ETL/Customers/Common/HCM/WorkStructuresMigration/WorkStructure_IFTY_V1_FUSN_R7/data-in/Fusion_Meta_Source.xlsx
+++ b/Fusion/ETL/Customers/Common/HCM/WorkStructuresMigration/WorkStructure_IFTY_V1_FUSN_R7/data-in/Fusion_Meta_Source.xlsx
@@ -4,19 +4,19 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Update Assignment" sheetId="1" r:id="rId1"/>
+    <sheet name="Create Work Rel Assignment" sheetId="2" r:id="rId2"/>
+    <sheet name="PersonPII" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="146">
   <si>
     <t>* Person Number</t>
   </si>
@@ -310,13 +310,157 @@
   </si>
   <si>
     <t>Assignment Attribute 6</t>
+  </si>
+  <si>
+    <t>* Work Relationship Start Date</t>
+  </si>
+  <si>
+    <t>Worker Number</t>
+  </si>
+  <si>
+    <t>* Worker Type</t>
+  </si>
+  <si>
+    <t>On Military Service</t>
+  </si>
+  <si>
+    <t>Termination Action</t>
+  </si>
+  <si>
+    <t>Termination Reason</t>
+  </si>
+  <si>
+    <t>Termination Date</t>
+  </si>
+  <si>
+    <t>* Legal Employer</t>
+  </si>
+  <si>
+    <t>Legal Employer Seniority Date</t>
+  </si>
+  <si>
+    <t>Enterprise Seniority Date</t>
+  </si>
+  <si>
+    <t>Work Relationship DDF Context</t>
+  </si>
+  <si>
+    <t>Work Relationship Legislative Information Number 1</t>
+  </si>
+  <si>
+    <t>Work Relationship Legislative Information Date 1</t>
+  </si>
+  <si>
+    <t>Work Relationship Legislative Information Date 2</t>
+  </si>
+  <si>
+    <t>Work Relationship Legislative Information Date 3</t>
+  </si>
+  <si>
+    <t>Work Relationship Legislative Information 1</t>
+  </si>
+  <si>
+    <t>Work Relationship Legislative Information 2</t>
+  </si>
+  <si>
+    <t>Work Relationship Legislative Information 3</t>
+  </si>
+  <si>
+    <t>Work Relationship Legislative Information 4</t>
+  </si>
+  <si>
+    <t>Work Relationship Legislative Information 5</t>
+  </si>
+  <si>
+    <t>Work Relationship Legislative Information 6</t>
+  </si>
+  <si>
+    <t>Work Relationship DFF Context</t>
+  </si>
+  <si>
+    <t>Work Relationship Attribute Number 1</t>
+  </si>
+  <si>
+    <t>Work Relationship Attribute Date 1</t>
+  </si>
+  <si>
+    <t>Work Relationship Attribute Date 2</t>
+  </si>
+  <si>
+    <t>Work Relationship Attribute Date 3</t>
+  </si>
+  <si>
+    <t>Work Relationship Attribute 1</t>
+  </si>
+  <si>
+    <t>Work Relationship Attribute 2</t>
+  </si>
+  <si>
+    <t>Work Relationship Attribute 3</t>
+  </si>
+  <si>
+    <t>Work Relationship Attribute 4</t>
+  </si>
+  <si>
+    <t>Work Relationship Attribute 5</t>
+  </si>
+  <si>
+    <t>Work Relationship Attribute 6</t>
+  </si>
+  <si>
+    <t>Assignment Number</t>
+  </si>
+  <si>
+    <t>Line Manager E-Mail</t>
+  </si>
+  <si>
+    <t>Salary Basis</t>
+  </si>
+  <si>
+    <t>Salary Amount</t>
+  </si>
+  <si>
+    <t>Current Employee Number</t>
+  </si>
+  <si>
+    <t>*Enterprise Start Date</t>
+  </si>
+  <si>
+    <t>Date of Birth</t>
+  </si>
+  <si>
+    <t>Country of Birth</t>
+  </si>
+  <si>
+    <t>Region of Birth</t>
+  </si>
+  <si>
+    <t>Town of Birth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Primary Identifier (Yes, No) </t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>National ID Type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ID Number </t>
+  </si>
+  <si>
+    <t>Issue Date</t>
+  </si>
+  <si>
+    <t>Expiration Date</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -330,8 +474,15 @@
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color indexed="9"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -344,8 +495,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="49"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -368,6 +525,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -375,10 +547,16 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyProtection="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" quotePrefix="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -677,7 +855,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:CT1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:CT1"/>
     </sheetView>
   </sheetViews>
@@ -986,24 +1164,443 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:DU1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="DC5" sqref="DC5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:125" ht="115.5">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="T1" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="U1" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="V1" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="W1" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="X1" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="Y1" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="Z1" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="AA1" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="AB1" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="AC1" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="AD1" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="AE1" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="AF1" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="AG1" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="AH1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="AI1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="AJ1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="AK1" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="AL1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="AM1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="AN1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="AO1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="AP1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="AQ1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AR1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AS1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="AT1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="AU1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="AV1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="AW1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="AX1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AY1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="AZ1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="BA1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="BB1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="BC1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="BD1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="BE1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="BF1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="BG1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="BH1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="BI1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="BJ1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="BK1" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="BL1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="BM1" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="BN1" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="BO1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="BP1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="BQ1" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="BR1" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="BS1" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="BT1" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="BU1" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="BV1" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="BW1" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="BX1" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="BY1" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="BZ1" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="CA1" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="CB1" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="CC1" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="CD1" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="CE1" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="CF1" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="CG1" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="CH1" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="CI1" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="CJ1" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="CK1" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="CL1" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="CM1" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="CN1" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="CO1" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="CP1" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="CQ1" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="CR1" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="CS1" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="CT1" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="CU1" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="CV1" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="CW1" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="CX1" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="CY1" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="CZ1" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="DA1" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="DB1" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="DC1" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="DD1" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="DE1" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="DF1" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="DG1" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="DH1" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="DI1" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="DJ1" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="DK1" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="DL1" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="DM1" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="DN1" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="DO1" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="DP1" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="DQ1" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="DR1" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="DS1" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="DT1" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="DU1" s="2" t="s">
+        <v>133</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:L1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:12" ht="38.25">
+      <c r="A1" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>145</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>